<commit_message>
New Phone, whose this
Modification of pipeline to save only full seurat rds and h5ad objects
Sorting of data to ensure cleanliness
Adding graphical summary and data tree
</commit_message>
<xml_diff>
--- a/summaryInfo/sample.directory.xlsx
+++ b/summaryInfo/sample.directory.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/Other computers/iMac/utility/summaryInfo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Documents/GitHub/utility/summaryInfo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2AF83798-5634-A040-BDBC-93BAF7FC4E06}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E57118-1158-134C-BCC5-A22C6CF1DEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13840" yWindow="10800" windowWidth="34580" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi6tBdJCFxaTgjtse94ZjZvYTMgNg=="/>
     </ext>
@@ -25,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8463" uniqueCount="1514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9551" uniqueCount="1708">
   <si>
     <t>SampleLabel</t>
   </si>
@@ -4567,6 +4577,588 @@
   </si>
   <si>
     <t>Neoadjuvant Chemotherapy + Pembrolizumab</t>
+  </si>
+  <si>
+    <t>CRLM08_PT</t>
+  </si>
+  <si>
+    <t>CRLM08_PN</t>
+  </si>
+  <si>
+    <t>CRLM08_LN</t>
+  </si>
+  <si>
+    <t>CRLM08_MT</t>
+  </si>
+  <si>
+    <t>CRLM08_MN</t>
+  </si>
+  <si>
+    <t>CRLM08_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM09_PT</t>
+  </si>
+  <si>
+    <t>CRLM09_PN</t>
+  </si>
+  <si>
+    <t>CRLM09_LN</t>
+  </si>
+  <si>
+    <t>CRLM09_MT</t>
+  </si>
+  <si>
+    <t>CRLM09_MN</t>
+  </si>
+  <si>
+    <t>CRLM09_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM10_PT</t>
+  </si>
+  <si>
+    <t>CRLM10_PN</t>
+  </si>
+  <si>
+    <t>CRLM10_LN</t>
+  </si>
+  <si>
+    <t>CRLM10_MT</t>
+  </si>
+  <si>
+    <t>CRLM10_MN</t>
+  </si>
+  <si>
+    <t>CRLM10_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM11_PT</t>
+  </si>
+  <si>
+    <t>CRLM11_PN</t>
+  </si>
+  <si>
+    <t>CRLM11_LN</t>
+  </si>
+  <si>
+    <t>CRLM11_MT</t>
+  </si>
+  <si>
+    <t>CRLM11_MN</t>
+  </si>
+  <si>
+    <t>CRLM11_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM12_PT</t>
+  </si>
+  <si>
+    <t>CRLM12_PN</t>
+  </si>
+  <si>
+    <t>CRLM12_LN</t>
+  </si>
+  <si>
+    <t>CRLM12_MT</t>
+  </si>
+  <si>
+    <t>CRLM12_MN</t>
+  </si>
+  <si>
+    <t>CRLM12_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM13_PT</t>
+  </si>
+  <si>
+    <t>CRLM13_PN</t>
+  </si>
+  <si>
+    <t>CRLM13_LN</t>
+  </si>
+  <si>
+    <t>CRLM13_MT</t>
+  </si>
+  <si>
+    <t>CRLM13_MN</t>
+  </si>
+  <si>
+    <t>CRLM13_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM14_PT</t>
+  </si>
+  <si>
+    <t>CRLM14_PN</t>
+  </si>
+  <si>
+    <t>CRLM14_LN</t>
+  </si>
+  <si>
+    <t>CRLM14_MT</t>
+  </si>
+  <si>
+    <t>CRLM14_MN</t>
+  </si>
+  <si>
+    <t>CRLM14_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM15_PT</t>
+  </si>
+  <si>
+    <t>CRLM15_PN</t>
+  </si>
+  <si>
+    <t>CRLM15_LN</t>
+  </si>
+  <si>
+    <t>CRLM15_MT</t>
+  </si>
+  <si>
+    <t>CRLM15_MN</t>
+  </si>
+  <si>
+    <t>CRLM15_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM16_PT</t>
+  </si>
+  <si>
+    <t>CRLM16_PN</t>
+  </si>
+  <si>
+    <t>CRLM16_LN</t>
+  </si>
+  <si>
+    <t>CRLM16_MT</t>
+  </si>
+  <si>
+    <t>CRLM16_MN</t>
+  </si>
+  <si>
+    <t>CRLM16_PBMC</t>
+  </si>
+  <si>
+    <t>CRLM17_PT</t>
+  </si>
+  <si>
+    <t>CRLM17_PN</t>
+  </si>
+  <si>
+    <t>CRLM17_LN</t>
+  </si>
+  <si>
+    <t>CRLM17_MT</t>
+  </si>
+  <si>
+    <t>CRLM17_MN</t>
+  </si>
+  <si>
+    <t>CRLM17_PBMC</t>
+  </si>
+  <si>
+    <t>CT4</t>
+  </si>
+  <si>
+    <t>CN4.1</t>
+  </si>
+  <si>
+    <t>CL4</t>
+  </si>
+  <si>
+    <t>CM4</t>
+  </si>
+  <si>
+    <t>CN4.2</t>
+  </si>
+  <si>
+    <t>CB4</t>
+  </si>
+  <si>
+    <t>CT5</t>
+  </si>
+  <si>
+    <t>CN5.1</t>
+  </si>
+  <si>
+    <t>CL5</t>
+  </si>
+  <si>
+    <t>CM5</t>
+  </si>
+  <si>
+    <t>CN5.2</t>
+  </si>
+  <si>
+    <t>CB5</t>
+  </si>
+  <si>
+    <t>CT6</t>
+  </si>
+  <si>
+    <t>CN6.1</t>
+  </si>
+  <si>
+    <t>CL6</t>
+  </si>
+  <si>
+    <t>CM6</t>
+  </si>
+  <si>
+    <t>CN6.2</t>
+  </si>
+  <si>
+    <t>CB6</t>
+  </si>
+  <si>
+    <t>CT7</t>
+  </si>
+  <si>
+    <t>CN7.1</t>
+  </si>
+  <si>
+    <t>CL7</t>
+  </si>
+  <si>
+    <t>CM7</t>
+  </si>
+  <si>
+    <t>CN7.2</t>
+  </si>
+  <si>
+    <t>CB7</t>
+  </si>
+  <si>
+    <t>CT8</t>
+  </si>
+  <si>
+    <t>CN8.1</t>
+  </si>
+  <si>
+    <t>CL8</t>
+  </si>
+  <si>
+    <t>CM8</t>
+  </si>
+  <si>
+    <t>CN8.2</t>
+  </si>
+  <si>
+    <t>CB8</t>
+  </si>
+  <si>
+    <t>CT9</t>
+  </si>
+  <si>
+    <t>CN9.1</t>
+  </si>
+  <si>
+    <t>CL9</t>
+  </si>
+  <si>
+    <t>CM9</t>
+  </si>
+  <si>
+    <t>CN9.2</t>
+  </si>
+  <si>
+    <t>CB9</t>
+  </si>
+  <si>
+    <t>CT10</t>
+  </si>
+  <si>
+    <t>CN10.1</t>
+  </si>
+  <si>
+    <t>CL10</t>
+  </si>
+  <si>
+    <t>CM10</t>
+  </si>
+  <si>
+    <t>CN10.2</t>
+  </si>
+  <si>
+    <t>CB10</t>
+  </si>
+  <si>
+    <t>CT11</t>
+  </si>
+  <si>
+    <t>CN11.1</t>
+  </si>
+  <si>
+    <t>CL11</t>
+  </si>
+  <si>
+    <t>CM11</t>
+  </si>
+  <si>
+    <t>CN11.2</t>
+  </si>
+  <si>
+    <t>CB11</t>
+  </si>
+  <si>
+    <t>CT12</t>
+  </si>
+  <si>
+    <t>CN12.1</t>
+  </si>
+  <si>
+    <t>CL12</t>
+  </si>
+  <si>
+    <t>CM12</t>
+  </si>
+  <si>
+    <t>CN12.2</t>
+  </si>
+  <si>
+    <t>CB12</t>
+  </si>
+  <si>
+    <t>CT13</t>
+  </si>
+  <si>
+    <t>CN13.1</t>
+  </si>
+  <si>
+    <t>CL13</t>
+  </si>
+  <si>
+    <t>CM13</t>
+  </si>
+  <si>
+    <t>CN13.2</t>
+  </si>
+  <si>
+    <t>CB13</t>
+  </si>
+  <si>
+    <t>GSE164522</t>
+  </si>
+  <si>
+    <t>Metastasis</t>
+  </si>
+  <si>
+    <t>Patient192</t>
+  </si>
+  <si>
+    <t>Patient193</t>
+  </si>
+  <si>
+    <t>Patient194</t>
+  </si>
+  <si>
+    <t>Patient195</t>
+  </si>
+  <si>
+    <t>Patient196</t>
+  </si>
+  <si>
+    <t>Patient197</t>
+  </si>
+  <si>
+    <t>Patient198</t>
+  </si>
+  <si>
+    <t>Patient199</t>
+  </si>
+  <si>
+    <t>Patient200</t>
+  </si>
+  <si>
+    <t>Patient201</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>Patient202</t>
+  </si>
+  <si>
+    <t>Patient203</t>
+  </si>
+  <si>
+    <t>Patient204</t>
+  </si>
+  <si>
+    <t>Patient205</t>
+  </si>
+  <si>
+    <t>Patient206</t>
+  </si>
+  <si>
+    <t>Patient207</t>
+  </si>
+  <si>
+    <t>Patient208</t>
+  </si>
+  <si>
+    <t>Patient209</t>
+  </si>
+  <si>
+    <t>T021518_TRM [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798827</t>
+  </si>
+  <si>
+    <t>T022719_TRM [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798828</t>
+  </si>
+  <si>
+    <t>T082219_TRM [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798829</t>
+  </si>
+  <si>
+    <t>T021518_ReCir [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798830</t>
+  </si>
+  <si>
+    <t>T022719_ReCir [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798832</t>
+  </si>
+  <si>
+    <t>T082219_ReCir [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798833</t>
+  </si>
+  <si>
+    <t>T042719CD8_2 [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798834</t>
+  </si>
+  <si>
+    <t>T042719CD8_3 [GEX]</t>
+  </si>
+  <si>
+    <t>GSM5798835</t>
+  </si>
+  <si>
+    <t>T041218-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828140</t>
+  </si>
+  <si>
+    <t>T051110-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828141</t>
+  </si>
+  <si>
+    <t>T051209-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828142</t>
+  </si>
+  <si>
+    <t>T072817-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828143</t>
+  </si>
+  <si>
+    <t>T042718-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828144</t>
+  </si>
+  <si>
+    <t>T021518-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828145</t>
+  </si>
+  <si>
+    <t>T022719-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828146</t>
+  </si>
+  <si>
+    <t>T082219-TRM-GEX</t>
+  </si>
+  <si>
+    <t>GSM5828147</t>
+  </si>
+  <si>
+    <t>GSE195486</t>
+  </si>
+  <si>
+    <t>Patient210</t>
+  </si>
+  <si>
+    <t>Patient211</t>
+  </si>
+  <si>
+    <t>Patient212</t>
+  </si>
+  <si>
+    <t>Patient213</t>
+  </si>
+  <si>
+    <t>OT7.1</t>
+  </si>
+  <si>
+    <t>OT7.2</t>
+  </si>
+  <si>
+    <t>OT8.1</t>
+  </si>
+  <si>
+    <t>OT8.2</t>
+  </si>
+  <si>
+    <t>OT9.1</t>
+  </si>
+  <si>
+    <t>OT9.2</t>
+  </si>
+  <si>
+    <t>OT10.1</t>
+  </si>
+  <si>
+    <t>OT10.2</t>
+  </si>
+  <si>
+    <t>OT11</t>
+  </si>
+  <si>
+    <t>OT12</t>
+  </si>
+  <si>
+    <t>OT13</t>
+  </si>
+  <si>
+    <t>OT14</t>
+  </si>
+  <si>
+    <t>OT15</t>
+  </si>
+  <si>
+    <t>OT16</t>
+  </si>
+  <si>
+    <t>OT17</t>
+  </si>
+  <si>
+    <t>OT18</t>
   </si>
 </sst>
 </file>
@@ -4625,337 +5217,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5189,8 +5451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S980"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E213" workbookViewId="0">
-      <selection activeCell="E11" sqref="E1:S1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="E498" sqref="E498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31499,101 +31761,3619 @@
         <v>229</v>
       </c>
     </row>
-    <row r="450" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A450" s="3" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B450" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C450" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D450" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E450" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F450" t="s">
+        <v>61</v>
+      </c>
+      <c r="G450" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H450" t="s">
+        <v>14</v>
+      </c>
+      <c r="I450" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J450" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K450" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L450" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M450" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N450" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="O450" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P450" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="451" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A451" s="3" t="s">
+        <v>1575</v>
+      </c>
+      <c r="B451" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C451" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D451" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E451" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F451" t="s">
+        <v>61</v>
+      </c>
+      <c r="G451" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H451" t="s">
+        <v>14</v>
+      </c>
+      <c r="I451" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J451" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K451" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L451" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M451" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N451" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="O451" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P451" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="452" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A452" s="3" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B452" t="s">
+        <v>1516</v>
+      </c>
+      <c r="C452" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D452" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E452" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F452" t="s">
+        <v>61</v>
+      </c>
+      <c r="G452" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H452" t="s">
+        <v>14</v>
+      </c>
+      <c r="I452" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J452" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K452" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L452" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M452" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N452" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="O452" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P452" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="453" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A453" s="3" t="s">
+        <v>1577</v>
+      </c>
+      <c r="B453" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C453" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D453" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E453" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F453" t="s">
+        <v>61</v>
+      </c>
+      <c r="G453" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H453" t="s">
+        <v>14</v>
+      </c>
+      <c r="I453" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J453" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K453" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L453" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M453" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N453" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="O453" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P453" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="454" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A454" s="3" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B454" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C454" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D454" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E454" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F454" t="s">
+        <v>61</v>
+      </c>
+      <c r="G454" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H454" t="s">
+        <v>14</v>
+      </c>
+      <c r="I454" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J454" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K454" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L454" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M454" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N454" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="O454" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P454" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="455" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A455" s="3" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B455" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C455" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D455" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E455" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F455" t="s">
+        <v>61</v>
+      </c>
+      <c r="G455" t="s">
+        <v>1636</v>
+      </c>
+      <c r="H455" t="s">
+        <v>14</v>
+      </c>
+      <c r="I455" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J455" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K455" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L455" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M455" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N455" s="3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="O455" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="P455" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="456" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A456" s="3" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C456" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D456" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E456" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F456" t="s">
+        <v>61</v>
+      </c>
+      <c r="G456" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H456" t="s">
+        <v>14</v>
+      </c>
+      <c r="I456" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J456" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K456" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L456" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M456" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N456" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O456" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P456" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="457" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A457" s="3" t="s">
+        <v>1581</v>
+      </c>
+      <c r="B457" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C457" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D457" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E457" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F457" t="s">
+        <v>61</v>
+      </c>
+      <c r="G457" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H457" t="s">
+        <v>14</v>
+      </c>
+      <c r="I457" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J457" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K457" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L457" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M457" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N457" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O457" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P457" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="458" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A458" s="3" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B458" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C458" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D458" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E458" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F458" t="s">
+        <v>61</v>
+      </c>
+      <c r="G458" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H458" t="s">
+        <v>14</v>
+      </c>
+      <c r="I458" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J458" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K458" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L458" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M458" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N458" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O458" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P458" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="459" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A459" s="3" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B459" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C459" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D459" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E459" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F459" t="s">
+        <v>61</v>
+      </c>
+      <c r="G459" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H459" t="s">
+        <v>14</v>
+      </c>
+      <c r="I459" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J459" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K459" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L459" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M459" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N459" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O459" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P459" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="460" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A460" s="3" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B460" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C460" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D460" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E460" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F460" t="s">
+        <v>61</v>
+      </c>
+      <c r="G460" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H460" t="s">
+        <v>14</v>
+      </c>
+      <c r="I460" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J460" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K460" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L460" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M460" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N460" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O460" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P460" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="461" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A461" s="3" t="s">
+        <v>1585</v>
+      </c>
+      <c r="B461" t="s">
+        <v>1525</v>
+      </c>
+      <c r="C461" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D461" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E461" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F461" t="s">
+        <v>61</v>
+      </c>
+      <c r="G461" t="s">
+        <v>1637</v>
+      </c>
+      <c r="H461" t="s">
+        <v>14</v>
+      </c>
+      <c r="I461" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J461" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K461" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L461" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M461" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N461" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O461" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P461" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="462" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A462" s="3" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B462" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C462" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D462" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E462" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F462" t="s">
+        <v>61</v>
+      </c>
+      <c r="G462" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H462" t="s">
+        <v>14</v>
+      </c>
+      <c r="I462" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J462" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K462" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L462" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M462" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N462" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O462" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P462" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="463" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A463" s="3" t="s">
+        <v>1587</v>
+      </c>
+      <c r="B463" t="s">
+        <v>1527</v>
+      </c>
+      <c r="C463" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D463" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E463" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F463" t="s">
+        <v>61</v>
+      </c>
+      <c r="G463" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H463" t="s">
+        <v>14</v>
+      </c>
+      <c r="I463" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J463" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K463" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L463" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M463" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N463" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O463" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P463" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="464" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A464" s="3" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B464" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C464" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D464" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E464" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F464" t="s">
+        <v>61</v>
+      </c>
+      <c r="G464" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H464" t="s">
+        <v>14</v>
+      </c>
+      <c r="I464" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J464" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K464" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L464" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M464" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N464" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O464" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P464" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="465" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A465" s="3" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B465" t="s">
+        <v>1529</v>
+      </c>
+      <c r="C465" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D465" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E465" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F465" t="s">
+        <v>61</v>
+      </c>
+      <c r="G465" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H465" t="s">
+        <v>14</v>
+      </c>
+      <c r="I465" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J465" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K465" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L465" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M465" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N465" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O465" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P465" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="466" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A466" s="3" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B466" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C466" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D466" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E466" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F466" t="s">
+        <v>61</v>
+      </c>
+      <c r="G466" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H466" t="s">
+        <v>14</v>
+      </c>
+      <c r="I466" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J466" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K466" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L466" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M466" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N466" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O466" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P466" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="467" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A467" s="3" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B467" t="s">
+        <v>1531</v>
+      </c>
+      <c r="C467" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D467" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E467" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F467" t="s">
+        <v>61</v>
+      </c>
+      <c r="G467" t="s">
+        <v>1638</v>
+      </c>
+      <c r="H467" t="s">
+        <v>14</v>
+      </c>
+      <c r="I467" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J467" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K467" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L467" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M467" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N467" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O467" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P467" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="468" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A468" s="3" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B468" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C468" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D468" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E468" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F468" t="s">
+        <v>61</v>
+      </c>
+      <c r="G468" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H468" t="s">
+        <v>14</v>
+      </c>
+      <c r="I468" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J468" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K468" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L468" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M468" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N468" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O468" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P468" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="469" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A469" s="3" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B469" t="s">
+        <v>1533</v>
+      </c>
+      <c r="C469" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D469" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E469" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F469" t="s">
+        <v>61</v>
+      </c>
+      <c r="G469" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H469" t="s">
+        <v>14</v>
+      </c>
+      <c r="I469" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J469" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K469" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L469" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M469" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N469" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O469" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P469" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="470" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A470" s="3" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B470" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C470" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D470" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E470" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F470" t="s">
+        <v>61</v>
+      </c>
+      <c r="G470" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H470" t="s">
+        <v>14</v>
+      </c>
+      <c r="I470" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J470" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K470" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L470" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M470" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N470" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O470" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P470" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="471" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A471" s="3" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B471" t="s">
+        <v>1535</v>
+      </c>
+      <c r="C471" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D471" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E471" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F471" t="s">
+        <v>61</v>
+      </c>
+      <c r="G471" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H471" t="s">
+        <v>14</v>
+      </c>
+      <c r="I471" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J471" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K471" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L471" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M471" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N471" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O471" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P471" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="472" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A472" s="3" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B472" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C472" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D472" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E472" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F472" t="s">
+        <v>61</v>
+      </c>
+      <c r="G472" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H472" t="s">
+        <v>14</v>
+      </c>
+      <c r="I472" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J472" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K472" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L472" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M472" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N472" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O472" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P472" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="473" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A473" s="3" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B473" t="s">
+        <v>1537</v>
+      </c>
+      <c r="C473" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D473" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E473" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F473" t="s">
+        <v>61</v>
+      </c>
+      <c r="G473" t="s">
+        <v>1639</v>
+      </c>
+      <c r="H473" t="s">
+        <v>14</v>
+      </c>
+      <c r="I473" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J473" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K473" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L473" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M473" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N473" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O473" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P473" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="474" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A474" s="3" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B474" s="3" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C474" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D474" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E474" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F474" t="s">
+        <v>61</v>
+      </c>
+      <c r="G474" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H474" t="s">
+        <v>14</v>
+      </c>
+      <c r="I474" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J474" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K474" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L474" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M474" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N474" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O474" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P474" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="475" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A475" s="3" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B475" s="3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="C475" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D475" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E475" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F475" t="s">
+        <v>61</v>
+      </c>
+      <c r="G475" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H475" t="s">
+        <v>14</v>
+      </c>
+      <c r="I475" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J475" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K475" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L475" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M475" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N475" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O475" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P475" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="476" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A476" s="3" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C476" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D476" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E476" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F476" t="s">
+        <v>61</v>
+      </c>
+      <c r="G476" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H476" t="s">
+        <v>14</v>
+      </c>
+      <c r="I476" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J476" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K476" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L476" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M476" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N476" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O476" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P476" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="477" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A477" s="3" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C477" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D477" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E477" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F477" t="s">
+        <v>61</v>
+      </c>
+      <c r="G477" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H477" t="s">
+        <v>14</v>
+      </c>
+      <c r="I477" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J477" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K477" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L477" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M477" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N477" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O477" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P477" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="478" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A478" s="3" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C478" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D478" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E478" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F478" t="s">
+        <v>61</v>
+      </c>
+      <c r="G478" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H478" t="s">
+        <v>14</v>
+      </c>
+      <c r="I478" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J478" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K478" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L478" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M478" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N478" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O478" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P478" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="479" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A479" s="3" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B479" s="3" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C479" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D479" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E479" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F479" t="s">
+        <v>61</v>
+      </c>
+      <c r="G479" t="s">
+        <v>1640</v>
+      </c>
+      <c r="H479" t="s">
+        <v>14</v>
+      </c>
+      <c r="I479" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J479" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K479" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L479" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M479" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N479" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O479" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P479" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="480" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A480" s="3" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B480" s="3" t="s">
+        <v>1544</v>
+      </c>
+      <c r="C480" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D480" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E480" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F480" t="s">
+        <v>61</v>
+      </c>
+      <c r="G480" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H480" t="s">
+        <v>14</v>
+      </c>
+      <c r="I480" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J480" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K480" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L480" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M480" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N480" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O480" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P480" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="481" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A481" s="3" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B481" s="3" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C481" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D481" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E481" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F481" t="s">
+        <v>61</v>
+      </c>
+      <c r="G481" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H481" t="s">
+        <v>14</v>
+      </c>
+      <c r="I481" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J481" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K481" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L481" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M481" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N481" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O481" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P481" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="482" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A482" s="3" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B482" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="C482" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D482" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E482" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F482" t="s">
+        <v>61</v>
+      </c>
+      <c r="G482" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H482" t="s">
+        <v>14</v>
+      </c>
+      <c r="I482" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J482" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K482" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L482" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M482" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N482" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O482" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P482" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="483" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A483" s="3" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B483" s="3" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C483" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D483" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E483" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F483" t="s">
+        <v>61</v>
+      </c>
+      <c r="G483" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H483" t="s">
+        <v>14</v>
+      </c>
+      <c r="I483" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J483" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K483" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L483" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M483" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N483" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O483" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P483" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="484" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A484" s="3" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B484" s="3" t="s">
+        <v>1548</v>
+      </c>
+      <c r="C484" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D484" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E484" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F484" t="s">
+        <v>61</v>
+      </c>
+      <c r="G484" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H484" t="s">
+        <v>14</v>
+      </c>
+      <c r="I484" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J484" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K484" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L484" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M484" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N484" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O484" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P484" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="485" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A485" s="3" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C485" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D485" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E485" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F485" t="s">
+        <v>61</v>
+      </c>
+      <c r="G485" t="s">
+        <v>1641</v>
+      </c>
+      <c r="H485" t="s">
+        <v>14</v>
+      </c>
+      <c r="I485" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J485" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K485" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L485" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M485" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="N485" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O485" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P485" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="486" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A486" s="3" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B486" s="3" t="s">
+        <v>1550</v>
+      </c>
+      <c r="C486" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D486" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E486" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F486" t="s">
+        <v>61</v>
+      </c>
+      <c r="G486" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H486" t="s">
+        <v>14</v>
+      </c>
+      <c r="I486" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J486" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K486" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L486" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M486" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N486" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O486" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P486" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="487" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A487" s="3" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B487" s="3" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C487" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D487" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E487" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F487" t="s">
+        <v>61</v>
+      </c>
+      <c r="G487" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H487" t="s">
+        <v>14</v>
+      </c>
+      <c r="I487" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J487" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K487" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L487" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M487" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N487" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O487" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P487" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="488" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A488" s="3" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B488" s="3" t="s">
+        <v>1552</v>
+      </c>
+      <c r="C488" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D488" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E488" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F488" t="s">
+        <v>61</v>
+      </c>
+      <c r="G488" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H488" t="s">
+        <v>14</v>
+      </c>
+      <c r="I488" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J488" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K488" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L488" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M488" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N488" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O488" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P488" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="489" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A489" s="3" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B489" s="3" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C489" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D489" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E489" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F489" t="s">
+        <v>61</v>
+      </c>
+      <c r="G489" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H489" t="s">
+        <v>14</v>
+      </c>
+      <c r="I489" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J489" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K489" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L489" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M489" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N489" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O489" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P489" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="490" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A490" s="3" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B490" s="3" t="s">
+        <v>1554</v>
+      </c>
+      <c r="C490" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D490" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E490" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F490" t="s">
+        <v>61</v>
+      </c>
+      <c r="G490" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H490" t="s">
+        <v>14</v>
+      </c>
+      <c r="I490" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J490" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K490" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L490" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M490" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N490" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O490" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P490" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="491" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A491" s="3" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B491" s="3" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C491" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D491" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E491" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F491" t="s">
+        <v>61</v>
+      </c>
+      <c r="G491" t="s">
+        <v>1642</v>
+      </c>
+      <c r="H491" t="s">
+        <v>14</v>
+      </c>
+      <c r="I491" s="3" t="s">
+        <v>1480</v>
+      </c>
+      <c r="J491" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K491" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L491" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M491" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N491" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O491" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P491" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="492" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A492" s="3" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B492" s="3" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C492" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D492" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E492" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F492" t="s">
+        <v>61</v>
+      </c>
+      <c r="G492" t="s">
+        <v>1643</v>
+      </c>
+      <c r="H492" t="s">
+        <v>14</v>
+      </c>
+      <c r="I492" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J492" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K492" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L492" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M492" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N492" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O492" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P492" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="493" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A493" s="3" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B493" s="3" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C493" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D493" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E493" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F493" t="s">
+        <v>61</v>
+      </c>
+      <c r="G493" t="s">
+        <v>1643</v>
+      </c>
+      <c r="H493" t="s">
+        <v>14</v>
+      </c>
+      <c r="I493" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J493" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K493" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L493" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M493" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N493" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O493" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P493" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="494" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A494" s="3" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B494" s="3" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C494" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D494" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E494" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F494" t="s">
+        <v>61</v>
+      </c>
+      <c r="G494" t="s">
+        <v>1643</v>
+      </c>
+      <c r="H494" t="s">
+        <v>14</v>
+      </c>
+      <c r="I494" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J494" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K494" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L494" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M494" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N494" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O494" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P494" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="495" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A495" s="3" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B495" s="3" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C495" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D495" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E495" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F495" t="s">
+        <v>61</v>
+      </c>
+      <c r="G495" t="s">
+        <v>1643</v>
+      </c>
+      <c r="H495" t="s">
+        <v>14</v>
+      </c>
+      <c r="I495" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J495" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K495" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L495" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M495" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N495" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O495" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P495" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="496" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A496" s="3" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B496" s="3" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C496" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D496" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E496" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F496" t="s">
+        <v>61</v>
+      </c>
+      <c r="G496" t="s">
+        <v>1643</v>
+      </c>
+      <c r="H496" t="s">
+        <v>14</v>
+      </c>
+      <c r="I496" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J496" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K496" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L496" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M496" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N496" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O496" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P496" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="497" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A497" s="3" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B497" s="3" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C497" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D497" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E497" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F497" t="s">
+        <v>61</v>
+      </c>
+      <c r="G497" t="s">
+        <v>1643</v>
+      </c>
+      <c r="H497" t="s">
+        <v>14</v>
+      </c>
+      <c r="I497" s="3" t="s">
+        <v>1477</v>
+      </c>
+      <c r="J497" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="K497" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L497" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M497" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N497" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O497" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P497" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="498" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A498" s="3" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B498" s="3" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C498" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D498" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E498" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F498" t="s">
+        <v>61</v>
+      </c>
+      <c r="G498" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H498" t="s">
+        <v>14</v>
+      </c>
+      <c r="I498" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="J498" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K498" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L498" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M498" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N498" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O498" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P498" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="499" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A499" s="3" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B499" s="3" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C499" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D499" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E499" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F499" t="s">
+        <v>61</v>
+      </c>
+      <c r="G499" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H499" t="s">
+        <v>14</v>
+      </c>
+      <c r="I499" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="J499" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K499" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L499" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M499" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N499" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O499" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P499" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="500" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A500" s="3" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B500" s="3" t="s">
+        <v>1564</v>
+      </c>
+      <c r="C500" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D500" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E500" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F500" t="s">
+        <v>61</v>
+      </c>
+      <c r="G500" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H500" t="s">
+        <v>14</v>
+      </c>
+      <c r="I500" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="J500" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K500" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L500" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M500" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N500" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O500" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P500" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="501" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A501" s="3" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B501" s="3" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C501" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D501" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E501" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F501" t="s">
+        <v>61</v>
+      </c>
+      <c r="G501" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H501" t="s">
+        <v>14</v>
+      </c>
+      <c r="I501" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="J501" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K501" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L501" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M501" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N501" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O501" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P501" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="502" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="3" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B502" s="3" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C502" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D502" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E502" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F502" t="s">
+        <v>61</v>
+      </c>
+      <c r="G502" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H502" t="s">
+        <v>14</v>
+      </c>
+      <c r="I502" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="J502" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K502" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L502" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M502" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N502" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O502" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P502" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="503" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A503" s="3" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B503" s="3" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C503" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D503" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E503" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F503" t="s">
+        <v>61</v>
+      </c>
+      <c r="G503" t="s">
+        <v>1644</v>
+      </c>
+      <c r="H503" t="s">
+        <v>14</v>
+      </c>
+      <c r="I503" s="3" t="s">
+        <v>1473</v>
+      </c>
+      <c r="J503" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K503" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L503" s="3" t="s">
+        <v>1460</v>
+      </c>
+      <c r="M503" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="N503" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O503" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P503" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="504" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A504" s="3" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B504" s="3" t="s">
+        <v>1568</v>
+      </c>
+      <c r="C504" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D504" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E504" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F504" t="s">
+        <v>61</v>
+      </c>
+      <c r="G504" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H504" t="s">
+        <v>14</v>
+      </c>
+      <c r="I504" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J504" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K504" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L504" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M504" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N504" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O504" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P504" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="505" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A505" s="3" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B505" s="3" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C505" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D505" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E505" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F505" t="s">
+        <v>61</v>
+      </c>
+      <c r="G505" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H505" t="s">
+        <v>14</v>
+      </c>
+      <c r="I505" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J505" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K505" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L505" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M505" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N505" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O505" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P505" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="506" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A506" s="3" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B506" s="3" t="s">
+        <v>1570</v>
+      </c>
+      <c r="C506" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D506" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E506" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F506" t="s">
+        <v>61</v>
+      </c>
+      <c r="G506" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H506" t="s">
+        <v>14</v>
+      </c>
+      <c r="I506" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J506" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K506" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L506" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M506" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N506" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O506" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P506" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="507" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A507" s="3" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B507" s="3" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C507" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D507" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E507" s="3" t="s">
+        <v>1635</v>
+      </c>
+      <c r="F507" t="s">
+        <v>61</v>
+      </c>
+      <c r="G507" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H507" t="s">
+        <v>14</v>
+      </c>
+      <c r="I507" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J507" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K507" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L507" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M507" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N507" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O507" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P507" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="508" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A508" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B508" s="3" t="s">
+        <v>1572</v>
+      </c>
+      <c r="C508" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D508" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E508" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F508" t="s">
+        <v>61</v>
+      </c>
+      <c r="G508" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H508" t="s">
+        <v>14</v>
+      </c>
+      <c r="I508" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J508" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K508" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L508" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M508" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N508" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O508" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P508" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="509" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A509" s="3" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B509" s="3" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C509" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D509" t="s">
+        <v>1634</v>
+      </c>
+      <c r="E509" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F509" t="s">
+        <v>61</v>
+      </c>
+      <c r="G509" t="s">
+        <v>1645</v>
+      </c>
+      <c r="H509" t="s">
+        <v>14</v>
+      </c>
+      <c r="I509" s="3" t="s">
+        <v>1475</v>
+      </c>
+      <c r="J509" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="K509" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="L509" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="M509" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="N509" s="3" t="s">
+        <v>1467</v>
+      </c>
+      <c r="O509" s="3" t="s">
+        <v>1646</v>
+      </c>
+      <c r="P509" s="3" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="510" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A510" s="3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C510" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="D510" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E510" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F510" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G510" t="s">
+        <v>1647</v>
+      </c>
+      <c r="H510" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I510" s="3"/>
+      <c r="J510" s="3"/>
+      <c r="K510" s="3"/>
+      <c r="L510" s="3"/>
+      <c r="M510" s="3"/>
+      <c r="N510" s="3"/>
+      <c r="O510" s="3"/>
+      <c r="P510" s="3"/>
+    </row>
+    <row r="511" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A511" s="3" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C511" s="1" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D511" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E511" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F511" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G511" t="s">
+        <v>1648</v>
+      </c>
+      <c r="H511" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I511" s="3"/>
+      <c r="J511" s="3"/>
+      <c r="K511" s="3"/>
+      <c r="L511" s="3"/>
+      <c r="M511" s="3"/>
+      <c r="N511" s="3"/>
+      <c r="O511" s="3"/>
+      <c r="P511" s="3"/>
+    </row>
+    <row r="512" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A512" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C512" s="1" t="s">
+        <v>1660</v>
+      </c>
+      <c r="D512" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E512" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F512" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G512" t="s">
+        <v>1649</v>
+      </c>
+      <c r="H512" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I512" s="3"/>
+      <c r="J512" s="3"/>
+      <c r="K512" s="3"/>
+      <c r="L512" s="3"/>
+      <c r="M512" s="3"/>
+      <c r="N512" s="3"/>
+      <c r="O512" s="3"/>
+      <c r="P512" s="3"/>
+    </row>
+    <row r="513" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A513" s="3" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C513" s="1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="D513" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E513" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F513" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G513" t="s">
+        <v>1647</v>
+      </c>
+      <c r="H513" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I513" s="3"/>
+      <c r="J513" s="3"/>
+      <c r="K513" s="3"/>
+      <c r="L513" s="3"/>
+      <c r="M513" s="3"/>
+      <c r="N513" s="3"/>
+      <c r="O513" s="3"/>
+      <c r="P513" s="3"/>
+    </row>
+    <row r="514" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A514" s="3" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C514" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D514" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E514" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F514" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G514" t="s">
+        <v>1648</v>
+      </c>
+      <c r="H514" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I514" s="3"/>
+      <c r="J514" s="3"/>
+      <c r="K514" s="3"/>
+      <c r="L514" s="3"/>
+      <c r="M514" s="3"/>
+      <c r="N514" s="3"/>
+      <c r="O514" s="3"/>
+      <c r="P514" s="3"/>
+    </row>
+    <row r="515" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A515" s="3" t="s">
+        <v>1697</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C515" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D515" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E515" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F515" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G515" t="s">
+        <v>1649</v>
+      </c>
+      <c r="H515" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I515" s="3"/>
+      <c r="J515" s="3"/>
+      <c r="K515" s="3"/>
+      <c r="L515" s="3"/>
+      <c r="M515" s="3"/>
+      <c r="N515" s="3"/>
+      <c r="O515" s="3"/>
+      <c r="P515" s="3"/>
+    </row>
+    <row r="516" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A516" s="3" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C516" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D516" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E516" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F516" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G516" t="s">
+        <v>1650</v>
+      </c>
+      <c r="H516" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I516" s="3"/>
+      <c r="J516" s="3"/>
+      <c r="K516" s="3"/>
+      <c r="L516" s="3"/>
+      <c r="M516" s="3"/>
+      <c r="N516" s="3"/>
+      <c r="O516" s="3"/>
+      <c r="P516" s="3"/>
+    </row>
+    <row r="517" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A517" s="3" t="s">
+        <v>1699</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C517" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D517" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E517" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F517" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G517" t="s">
+        <v>1650</v>
+      </c>
+      <c r="H517" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I517" s="3"/>
+      <c r="J517" s="3"/>
+      <c r="K517" s="3"/>
+      <c r="L517" s="3"/>
+      <c r="M517" s="3"/>
+      <c r="N517" s="3"/>
+      <c r="O517" s="3"/>
+      <c r="P517" s="3"/>
+    </row>
+    <row r="518" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A518" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C518" s="1" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D518" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E518" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F518" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G518" t="s">
+        <v>1651</v>
+      </c>
+      <c r="H518" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I518" s="3"/>
+      <c r="J518" s="3"/>
+      <c r="K518" s="3"/>
+      <c r="L518" s="3"/>
+      <c r="M518" s="3"/>
+      <c r="N518" s="3"/>
+      <c r="O518" s="3"/>
+      <c r="P518" s="3"/>
+    </row>
+    <row r="519" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A519" s="3" t="s">
+        <v>1701</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C519" s="1" t="s">
+        <v>1674</v>
+      </c>
+      <c r="D519" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E519" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F519" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G519" t="s">
+        <v>1652</v>
+      </c>
+      <c r="H519" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I519" s="3"/>
+      <c r="J519" s="3"/>
+      <c r="K519" s="3"/>
+      <c r="L519" s="3"/>
+      <c r="M519" s="3"/>
+      <c r="N519" s="3"/>
+      <c r="O519" s="3"/>
+      <c r="P519" s="3"/>
+    </row>
+    <row r="520" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A520" s="3" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C520" s="1" t="s">
+        <v>1676</v>
+      </c>
+      <c r="D520" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E520" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F520" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G520" t="s">
+        <v>1653</v>
+      </c>
+      <c r="H520" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I520" s="3"/>
+      <c r="J520" s="3"/>
+      <c r="K520" s="3"/>
+      <c r="L520" s="3"/>
+      <c r="M520" s="3"/>
+      <c r="N520" s="3"/>
+      <c r="O520" s="3"/>
+      <c r="P520" s="3"/>
+    </row>
+    <row r="521" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A521" s="3" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C521" s="1" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D521" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E521" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F521" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G521" t="s">
+        <v>1654</v>
+      </c>
+      <c r="H521" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I521" s="3"/>
+      <c r="J521" s="3"/>
+      <c r="K521" s="3"/>
+      <c r="L521" s="3"/>
+      <c r="M521" s="3"/>
+      <c r="N521" s="3"/>
+      <c r="O521" s="3"/>
+      <c r="P521" s="3"/>
+    </row>
+    <row r="522" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A522" s="3" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C522" s="1" t="s">
+        <v>1680</v>
+      </c>
+      <c r="D522" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E522" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F522" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G522" t="s">
+        <v>1688</v>
+      </c>
+      <c r="H522" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I522" s="3"/>
+      <c r="J522" s="3"/>
+      <c r="K522" s="3"/>
+      <c r="L522" s="3"/>
+      <c r="M522" s="3"/>
+      <c r="N522" s="3"/>
+      <c r="O522" s="3"/>
+      <c r="P522" s="3"/>
+    </row>
+    <row r="523" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A523" s="3" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C523" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D523" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E523" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F523" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G523" t="s">
+        <v>1689</v>
+      </c>
+      <c r="H523" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I523" s="3"/>
+      <c r="J523" s="3"/>
+      <c r="K523" s="3"/>
+      <c r="L523" s="3"/>
+      <c r="M523" s="3"/>
+      <c r="N523" s="3"/>
+      <c r="O523" s="3"/>
+      <c r="P523" s="3"/>
+    </row>
+    <row r="524" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A524" s="3" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C524" s="1" t="s">
+        <v>1684</v>
+      </c>
+      <c r="D524" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E524" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F524" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G524" t="s">
+        <v>1690</v>
+      </c>
+      <c r="H524" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I524" s="3"/>
+      <c r="J524" s="3"/>
+      <c r="K524" s="3"/>
+      <c r="L524" s="3"/>
+      <c r="M524" s="3"/>
+      <c r="N524" s="3"/>
+      <c r="O524" s="3"/>
+      <c r="P524" s="3"/>
+    </row>
+    <row r="525" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A525" s="3" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C525" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D525" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E525" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F525" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G525" t="s">
+        <v>1691</v>
+      </c>
+      <c r="H525" s="3" t="s">
+        <v>772</v>
+      </c>
+      <c r="I525" s="3"/>
+      <c r="J525" s="3"/>
+      <c r="K525" s="3"/>
+      <c r="L525" s="3"/>
+      <c r="M525" s="3"/>
+      <c r="N525" s="3"/>
+      <c r="O525" s="3"/>
+      <c r="P525" s="3"/>
+    </row>
+    <row r="526" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A526" s="3"/>
+    </row>
+    <row r="527" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B527" s="1"/>
+      <c r="C527" s="1"/>
+    </row>
+    <row r="528" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B528" s="1"/>
+      <c r="C528" s="1"/>
+    </row>
+    <row r="529" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B529" s="1"/>
+      <c r="C529" s="1"/>
+    </row>
+    <row r="530" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B530" s="1"/>
+      <c r="C530" s="1"/>
+    </row>
+    <row r="531" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B531" s="1"/>
+      <c r="C531" s="1"/>
+    </row>
+    <row r="532" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B532" s="1"/>
+      <c r="C532" s="1"/>
+    </row>
+    <row r="533" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B533" s="1"/>
+      <c r="C533" s="1"/>
+    </row>
+    <row r="534" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B534" s="1"/>
+      <c r="C534" s="1"/>
+    </row>
+    <row r="535" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B535" s="1"/>
+      <c r="C535" s="1"/>
+    </row>
+    <row r="536" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B536" s="1"/>
+      <c r="C536" s="1"/>
+    </row>
+    <row r="537" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B537" s="1"/>
+      <c r="C537" s="1"/>
+    </row>
+    <row r="538" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B538" s="1"/>
+      <c r="C538" s="1"/>
+    </row>
+    <row r="539" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B539" s="1"/>
+      <c r="C539" s="1"/>
+    </row>
+    <row r="540" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B540" s="1"/>
+      <c r="C540" s="1"/>
+    </row>
+    <row r="541" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B541" s="1"/>
+      <c r="C541" s="1"/>
+    </row>
+    <row r="542" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B542" s="1"/>
+      <c r="C542" s="1"/>
+    </row>
+    <row r="543" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32033,10 +35813,10 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:A1048576">
-    <cfRule type="duplicateValues" dxfId="34" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="33" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="36"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>